<commit_message>
Updated everything for basic stats analysis
</commit_message>
<xml_diff>
--- a/basic_stats_output.xlsx
+++ b/basic_stats_output.xlsx
@@ -13,17 +13,18 @@
     <sheet name="Head to Head Scores" sheetId="4" r:id="rId4"/>
     <sheet name="Highest Scores" sheetId="5" r:id="rId5"/>
     <sheet name="Lowest Scores" sheetId="6" r:id="rId6"/>
-    <sheet name="Made Playoffs" sheetId="7" r:id="rId7"/>
-    <sheet name="Made Losers Bowl" sheetId="8" r:id="rId8"/>
-    <sheet name="Average Regular Season Finish" sheetId="9" r:id="rId9"/>
-    <sheet name="Average Final Finish" sheetId="10" r:id="rId10"/>
+    <sheet name="Largest Victories" sheetId="7" r:id="rId7"/>
+    <sheet name="Made Playoffs" sheetId="8" r:id="rId8"/>
+    <sheet name="Made Losers Bowl" sheetId="9" r:id="rId9"/>
+    <sheet name="Average Regular Season Finish" sheetId="10" r:id="rId10"/>
+    <sheet name="Average Final Finish" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="355">
   <si>
     <t>Year</t>
   </si>
@@ -1015,6 +1016,9 @@
     <t>Week 1</t>
   </si>
   <si>
+    <t>Margin</t>
+  </si>
+  <si>
     <t>True</t>
   </si>
   <si>
@@ -1027,10 +1031,10 @@
     <t>4 / 11</t>
   </si>
   <si>
-    <t>6 / 9</t>
-  </si>
-  <si>
-    <t>6 / 11</t>
+    <t>5 / 9</t>
+  </si>
+  <si>
+    <t>5 / 11</t>
   </si>
   <si>
     <t>3 / 11</t>
@@ -1039,10 +1043,10 @@
     <t>3 / 9</t>
   </si>
   <si>
-    <t>5 / 11</t>
-  </si>
-  <si>
-    <t>8 / 11</t>
+    <t>7 / 11</t>
+  </si>
+  <si>
+    <t>Check</t>
   </si>
   <si>
     <t>2 / 11</t>
@@ -1052,9 +1056,6 @@
   </si>
   <si>
     <t>1 / 9</t>
-  </si>
-  <si>
-    <t>0 / 11</t>
   </si>
   <si>
     <t>Most Common</t>
@@ -1972,6 +1973,504 @@
         <v>345</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A3" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A4" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A5" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A7" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A8" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A9" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A10" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A11" s="2">
+        <v>2023</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A12" s="2">
+        <v>2024</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5.45</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4.91</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4.11</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5.45</v>
+      </c>
+      <c r="F13" s="2">
+        <v>6.36</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5.22</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5.73</v>
+      </c>
+      <c r="I13" s="2">
+        <v>4.64</v>
+      </c>
+      <c r="J13" s="2">
+        <v>3.73</v>
+      </c>
+      <c r="K13" s="2">
+        <v>5.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="11" width="12.85546875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>348</v>
       </c>
       <c r="D2" s="4"/>
@@ -3795,7 +4294,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="1">
-        <v>-10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="18" customHeight="1">
@@ -3827,7 +4326,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="1">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" ht="18" customHeight="1">
@@ -3859,7 +4358,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="1">
-        <v>-27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" ht="18" customHeight="1">
@@ -3923,7 +4422,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="1">
-        <v>-8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="18" customHeight="1">
@@ -3955,7 +4454,7 @@
         <v>3</v>
       </c>
       <c r="K7" s="1">
-        <v>-19</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="18" customHeight="1">
@@ -3987,7 +4486,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="1">
-        <v>86</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" ht="18" customHeight="1">
@@ -4019,7 +4518,7 @@
         <v>4</v>
       </c>
       <c r="K9" s="1">
-        <v>-46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" ht="18" customHeight="1">
@@ -4051,7 +4550,7 @@
         <v>6</v>
       </c>
       <c r="K10" s="1">
-        <v>-9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" ht="18" customHeight="1">
@@ -4083,7 +4582,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="1">
-        <v>-22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" ht="18" customHeight="1">
@@ -5061,7 +5560,675 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="11" width="21.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>93.47999999999999</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2017</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>90.22000000000001</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2015</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>85.30000000000001</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>80.89999999999999</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2016</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>80.75999999999999</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>-93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>79.74000000000001</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>79.11999999999999</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>78.88000000000001</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>77.86000000000001</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1">
+        <v>4</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+      <c r="K10" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>76.72</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1">
+        <v>4</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>75.66000000000001</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>74.76000000000001</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>74.14000000000001</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>73.26000000000001</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>73.12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>73.06000000000002</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>73.04000000000001</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>72.47999999999999</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>71.14</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>69.44</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>67.72</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>67.55999999999999</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>67.33999999999999</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>67.31999999999999</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5070,7 +6237,7 @@
     <col min="1" max="11" width="12.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5104,417 +6271,453 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L1" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="2">
         <v>2014</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>330</v>
+      <c r="B2" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="I2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="2">
         <v>2015</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>330</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>330</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>330</v>
+      <c r="J3" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="2">
         <v>2016</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>330</v>
+      <c r="B4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L4" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="D5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="F5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="2">
         <v>2018</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>330</v>
+      <c r="F6" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="2">
         <v>2019</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>330</v>
+      <c r="B7" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="E7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="2">
         <v>2020</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="J8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="2">
         <v>2021</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>330</v>
+      <c r="B9" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="I9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="K9" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="2">
         <v>2022</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="D10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="F10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="J10" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="2">
         <v>2023</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="H11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="K11" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="2">
         <v>2024</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>330</v>
+      <c r="F12" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="G12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="K12" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>332</v>
+      </c>
+      <c r="L12" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>339</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -5522,9 +6725,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5533,7 +6736,7 @@
     <col min="1" max="11" width="12.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5567,915 +6770,453 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L1" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="2">
         <v>2014</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="F2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>331</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="2">
         <v>2015</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="2">
         <v>2016</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="J4" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>330</v>
+      <c r="B5" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="I5" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="2">
         <v>2018</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="2">
         <v>2019</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="F7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="2">
         <v>2020</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="2">
         <v>2021</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="G9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="L9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="2">
         <v>2022</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="2">
         <v>2023</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>330</v>
+      <c r="B11" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
+        <v>332</v>
+      </c>
+      <c r="L11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="2">
         <v>2024</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="D12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="I12" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>332</v>
+      </c>
+      <c r="L12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>336</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>341</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="11" width="12.85546875" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A2" s="2">
-        <v>2014</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A3" s="2">
-        <v>2015</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A4" s="2">
-        <v>2016</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A5" s="2">
-        <v>2017</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A6" s="2">
-        <v>2018</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="2">
-        <v>2019</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="2">
-        <v>2020</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="2">
-        <v>2021</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A10" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A11" s="2">
-        <v>2023</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A12" s="2">
-        <v>2024</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="2">
-        <v>5.45</v>
-      </c>
-      <c r="C13" s="2">
-        <v>4.91</v>
-      </c>
-      <c r="D13" s="2">
-        <v>4.11</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5.45</v>
-      </c>
-      <c r="F13" s="2">
-        <v>6.36</v>
-      </c>
-      <c r="G13" s="2">
-        <v>5.22</v>
-      </c>
-      <c r="H13" s="2">
-        <v>5.73</v>
-      </c>
-      <c r="I13" s="2">
-        <v>4.64</v>
-      </c>
-      <c r="J13" s="2">
-        <v>3.73</v>
-      </c>
-      <c r="K13" s="2">
-        <v>5.36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B14" s="2">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>4</v>
-      </c>
-      <c r="F14" s="2">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2">
-        <v>2</v>
-      </c>
-      <c r="H14" s="2">
-        <v>3</v>
-      </c>
-      <c r="I14" s="2">
-        <v>5</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2">
-        <v>2</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated everything for v2.0 of pt 1: basic stats analysis
</commit_message>
<xml_diff>
--- a/basic_stats_output.xlsx
+++ b/basic_stats_output.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="355">
   <si>
     <t>Year</t>
   </si>
@@ -4898,7 +4898,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="11" width="21.42578125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="21.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -5560,16 +5560,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="11" width="21.42578125" style="1" customWidth="1"/>
+    <col min="10" max="13" width="21.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>306</v>
       </c>
@@ -5580,28 +5580,34 @@
         <v>308</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5611,29 +5617,35 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2">
+        <v>158.2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2">
+        <v>64.72</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="F2" s="1">
+      <c r="H2" s="1">
         <v>2017</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1">
-        <v>4</v>
-      </c>
-      <c r="J2" s="1">
-        <v>2</v>
+      <c r="J2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1">
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5643,29 +5655,35 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3">
+        <v>164.3</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3">
+        <v>74.08</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1">
         <v>2015</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="1">
-        <v>4</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="1">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1">
         <v>-11</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5675,29 +5693,35 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4">
+        <v>165.52</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4">
+        <v>80.22</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>2020</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="1">
-        <v>4</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2</v>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5707,29 +5731,35 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5">
+        <v>150.14</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5">
+        <v>69.23999999999999</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="F5" s="1">
+      <c r="H5" s="1">
         <v>2016</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="J5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="1">
-        <v>2</v>
-      </c>
       <c r="K5" s="1">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5739,29 +5769,35 @@
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6">
+        <v>141.88</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6">
+        <v>61.12</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="F6" s="1">
+      <c r="H6" s="1">
         <v>2024</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="1">
-        <v>4</v>
-      </c>
-      <c r="J6" s="1">
-        <v>2</v>
+      <c r="J6" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1">
         <v>-93</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -5771,29 +5807,35 @@
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7">
+        <v>142.74</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7">
+        <v>63</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H7" s="1">
         <v>2023</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="1">
-        <v>4</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
         <v>2</v>
       </c>
-      <c r="K7" s="1">
+      <c r="M7" s="1">
         <v>-17</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -5803,29 +5845,35 @@
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8">
+        <v>177.98</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8">
+        <v>98.86</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="F8" s="1">
+      <c r="H8" s="1">
         <v>2020</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="1">
-        <v>4</v>
-      </c>
-      <c r="J8" s="1">
-        <v>2</v>
+      <c r="J8" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="K8" s="1">
+        <v>5</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -5835,29 +5883,35 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9">
+        <v>145.36</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9">
+        <v>66.48</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="F9" s="1">
+      <c r="H9" s="1">
         <v>2019</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="J9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1">
         <v>4</v>
       </c>
-      <c r="J9" s="1">
-        <v>2</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="M9" s="1">
         <v>-26</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -5867,29 +5921,35 @@
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10">
+        <v>133.84</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10">
+        <v>55.98</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <v>2024</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="J10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="1">
         <v>4</v>
       </c>
-      <c r="J10" s="1">
+      <c r="L10" s="1">
         <v>2</v>
       </c>
-      <c r="K10" s="1">
+      <c r="M10" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:13">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -5899,29 +5959,35 @@
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11">
+        <v>142.78</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11">
+        <v>66.06</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="F11" s="1">
+      <c r="H11" s="1">
         <v>2019</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="1">
+      <c r="K11" s="1">
         <v>4</v>
       </c>
-      <c r="J11" s="1">
+      <c r="L11" s="1">
         <v>2</v>
       </c>
-      <c r="K11" s="1">
+      <c r="M11" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:13">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -5931,17 +5997,23 @@
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12">
+        <v>135.86</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12">
+        <v>60.2</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="F12" s="1">
+      <c r="H12" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -5951,17 +6023,23 @@
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13">
+        <v>146.12</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13">
+        <v>71.36</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="F13" s="1">
+      <c r="H13" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:13">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -5971,17 +6049,23 @@
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14">
+        <v>160.3</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14">
+        <v>85.90000000000001</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="F14" s="1">
+      <c r="H14" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:13">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -5991,17 +6075,23 @@
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15">
+        <v>143.74</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15">
+        <v>69.59999999999999</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="F15" s="1">
+      <c r="H15" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:13">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -6011,17 +6101,23 @@
       <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16">
+        <v>127.06</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16">
+        <v>53.8</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F16" s="1">
+      <c r="H16" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:8">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -6031,17 +6127,23 @@
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17">
+        <v>144.74</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17">
+        <v>71.62</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F17" s="1">
+      <c r="H17" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:8">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -6051,17 +6153,23 @@
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18">
+        <v>143.86</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18">
+        <v>70.8</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="F18" s="1">
+      <c r="H18" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:8">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -6071,17 +6179,23 @@
       <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19">
+        <v>174.96</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19">
+        <v>101.92</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="F19" s="1">
+      <c r="H19" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:8">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -6091,17 +6205,23 @@
       <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20">
+        <v>163.04</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20">
+        <v>90.56</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="F20" s="1">
+      <c r="H20" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:8">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -6111,17 +6231,23 @@
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21">
+        <v>136.38</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21">
+        <v>65.23999999999999</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="F21" s="1">
+      <c r="H21" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:8">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -6131,17 +6257,23 @@
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22">
+        <v>149.72</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22">
+        <v>80.28</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="F22" s="1">
+      <c r="H22" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:8">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -6151,17 +6283,23 @@
       <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23">
+        <v>132.9</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23">
+        <v>65.18000000000001</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="F23" s="1">
+      <c r="H23" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -6171,17 +6309,23 @@
       <c r="C24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24">
+        <v>162.32</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24">
+        <v>94.76000000000001</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="F24" s="1">
+      <c r="H24" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -6191,17 +6335,23 @@
       <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25">
+        <v>162.92</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25">
+        <v>95.58</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="F25" s="1">
+      <c r="H25" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:8">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -6211,13 +6361,19 @@
       <c r="C26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26">
+        <v>138.7</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26">
+        <v>71.38</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="F26" s="1">
+      <c r="H26" s="1">
         <v>2020</v>
       </c>
     </row>

</xml_diff>